<commit_message>
primer mvp, planilla completa
</commit_message>
<xml_diff>
--- a/planilla_base.xlsx
+++ b/planilla_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\ph_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3317829-CB50-4F37-B93D-A4C7A04DD252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D873698-7594-4B4C-8334-1254C450A00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="100" windowWidth="19190" windowHeight="10070" tabRatio="705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="3570" windowWidth="19185" windowHeight="10065" tabRatio="705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="33" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>BARRIO:</t>
   </si>
   <si>
-    <t>CIRC.:</t>
-  </si>
-  <si>
     <t>VTIERRA</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>VTOTAL</t>
+  </si>
+  <si>
+    <t>CIRCUNSCRIPCIÓN:</t>
   </si>
 </sst>
 </file>
@@ -196,7 +196,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-2C0A]\ #,##0.00"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -272,7 +272,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -555,19 +555,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -670,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -689,22 +676,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -719,67 +694,46 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -788,14 +742,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,14 +756,116 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -823,9 +873,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -838,98 +885,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1272,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1292,8 +1252,8 @@
     <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
     <col min="18" max="18" width="10.42578125" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" customWidth="1"/>
@@ -1301,22 +1261,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1330,8 +1290,8 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" spans="2:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -1342,15 +1302,15 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
-      <c r="N2" s="78" t="s">
+      <c r="N2" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="57"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="78"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1359,27 +1319,27 @@
       <c r="X2" s="2"/>
     </row>
     <row r="3" spans="2:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="81" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="60" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="46"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="34"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -1388,25 +1348,25 @@
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="82" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="44"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="33"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -1415,20 +1375,20 @@
       <c r="X4" s="2"/>
     </row>
     <row r="5" spans="2:24" ht="27.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
       <c r="N5" s="11" t="s">
         <v>40</v>
       </c>
@@ -1453,34 +1413,34 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="53" t="s">
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="53" t="s">
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="53" t="s">
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="45"/>
+      <c r="S7" s="82"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -1497,24 +1457,24 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="2:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
       <c r="R9" s="6"/>
       <c r="S9" s="7"/>
       <c r="T9" s="2"/>
@@ -1524,36 +1484,36 @@
       <c r="X9" s="2"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="71" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="71" t="s">
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="86"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="61"/>
       <c r="O10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="87" t="s">
+      <c r="Q10" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="87"/>
-      <c r="S10" s="88"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="63"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
@@ -1561,25 +1521,25 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="2:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="89" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="P11" s="91" t="s">
+      <c r="P11" s="66" t="s">
         <v>22</v>
       </c>
       <c r="Q11" s="5" t="s">
@@ -1598,13 +1558,13 @@
       <c r="X11" s="2"/>
     </row>
     <row r="12" spans="2:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="57" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1637,15 +1597,15 @@
       <c r="N12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O12" s="90"/>
-      <c r="P12" s="91"/>
-      <c r="Q12" s="92" t="s">
+      <c r="O12" s="65"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="92" t="s">
+      <c r="R12" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="S12" s="74" t="s">
+      <c r="S12" s="46" t="s">
         <v>29</v>
       </c>
       <c r="T12" s="2"/>
@@ -1655,44 +1615,44 @@
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="66"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="63" t="s">
+      <c r="B13" s="70"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="63" t="s">
+      <c r="F13" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="63" t="s">
+      <c r="G13" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="63" t="s">
+      <c r="H13" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="63" t="s">
+      <c r="I13" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="63" t="s">
+      <c r="J13" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="63" t="s">
+      <c r="K13" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="63" t="s">
+      <c r="L13" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="63" t="s">
+      <c r="M13" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="N13" s="63" t="s">
+      <c r="N13" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="90"/>
-      <c r="P13" s="91"/>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="92"/>
-      <c r="S13" s="74"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="46"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
@@ -1700,24 +1660,24 @@
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="67"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="75"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="64"/>
+      <c r="Q14" s="68"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="47"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
@@ -1725,105 +1685,105 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="24"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="41"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="25"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="55"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="43"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="25"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="55"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="43"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="25"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="36"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="43"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
@@ -1831,234 +1791,234 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="25"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="36"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="83"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="43"/>
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="25"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="36"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="43"/>
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="25"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="36"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="43"/>
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="25"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="36"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="43"/>
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="25"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="36"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="42"/>
+      <c r="S23" s="43"/>
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="25"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="36"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="43"/>
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="25"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="36"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="83"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="43"/>
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="25"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="36"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="83"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="43"/>
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="36"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="83"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="43"/>
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="41"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="36"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="83"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="43"/>
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="42"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="38"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="84"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="45"/>
     </row>
     <row r="30" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
@@ -2241,7 +2201,25 @@
       <c r="Q39" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="S12:S14"/>
     <mergeCell ref="B1:C4"/>
     <mergeCell ref="D1:M1"/>
@@ -2258,23 +2236,6 @@
     <mergeCell ref="P11:P14"/>
     <mergeCell ref="Q12:Q14"/>
     <mergeCell ref="R12:R14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E7:H7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
limpiar campos, arreglos en planilla base
</commit_message>
<xml_diff>
--- a/planilla_base.xlsx
+++ b/planilla_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\ph_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53391BEA-B46F-4239-8EE4-C9857FE627AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77DD4ED-87DC-49B1-8B47-60B43B530A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="375" windowWidth="28785" windowHeight="15105" tabRatio="705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">PROVINCIA  DE JUJUY                    </t>
   </si>
@@ -31,12 +31,6 @@
     <t>PADRON</t>
   </si>
   <si>
-    <t>U. FUNC.</t>
-  </si>
-  <si>
-    <t>POLIGONO</t>
-  </si>
-  <si>
     <t>VALOR DEL EDIFICIO</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>DECRETO O RESOLUCIÓN N°</t>
   </si>
   <si>
-    <t>Totales           (Col. 6 + 10)</t>
-  </si>
-  <si>
     <t>ANTES DE LLENAR ESTE FORMULARIO LÉASE LAS INSTRUCCIONES</t>
   </si>
   <si>
@@ -164,6 +155,18 @@
   </si>
   <si>
     <t>VTOTAL</t>
+  </si>
+  <si>
+    <t>U. Func.</t>
+  </si>
+  <si>
+    <t>Polígono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totales </t>
+  </si>
+  <si>
+    <t>(Col. 6 + 10)</t>
   </si>
 </sst>
 </file>
@@ -289,26 +292,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -430,17 +413,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -626,6 +598,43 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -633,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -643,229 +652,242 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1209,14 +1231,14 @@
   <dimension ref="B1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E18:E19"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
     <col min="6" max="6" width="6.85546875" customWidth="1"/>
@@ -1228,31 +1250,31 @@
     <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
     <col min="18" max="18" width="10.42578125" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" customWidth="1"/>
     <col min="20" max="23" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1266,25 +1288,25 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" spans="2:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="78"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="80"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="75"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="77"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1293,27 +1315,27 @@
       <c r="X2" s="2"/>
     </row>
     <row r="3" spans="2:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="44" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="31"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="28"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -1322,25 +1344,25 @@
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="30"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="27"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -1348,27 +1370,27 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="2:24" ht="27.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
+    <row r="5" spans="2:24" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -1387,24 +1409,24 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="46"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -1421,26 +1443,26 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="2:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="7"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="80"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
@@ -1448,34 +1470,34 @@
       <c r="X9" s="2"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B10" s="81"/>
-      <c r="C10" s="82"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
+        <v>3</v>
+      </c>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
       <c r="K10" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="70"/>
-      <c r="O10" s="5" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="85" t="s">
+        <v>18</v>
       </c>
       <c r="P10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="R10" s="71"/>
-      <c r="S10" s="72"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="61"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
@@ -1483,33 +1505,31 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="2:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="73" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="75" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="R11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="S11" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -1518,55 +1538,57 @@
       <c r="X11" s="2"/>
     </row>
     <row r="12" spans="2:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="52" t="s">
-        <v>3</v>
+      <c r="C12" s="69" t="s">
+        <v>45</v>
       </c>
       <c r="D12" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="F12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O12" s="74"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="76" t="s">
+      <c r="O12" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="76" t="s">
+      <c r="S12" s="44" t="s">
         <v>27</v>
-      </c>
-      <c r="S12" s="58" t="s">
-        <v>29</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
@@ -1575,44 +1597,46 @@
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="50"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="47" t="s">
+      <c r="B13" s="67"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="47" t="s">
+      <c r="M13" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="74"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="58"/>
+      <c r="N13" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="44"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
@@ -1620,24 +1644,24 @@
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="51"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="77"/>
-      <c r="S14" s="59"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="45"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
@@ -1645,105 +1669,105 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="36"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="38"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="33"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="38"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="33"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="15"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="38"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="33"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
@@ -1751,234 +1775,234 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="38"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="33"/>
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="15"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="38"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="33"/>
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="38"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="33"/>
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="15"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="38"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="33"/>
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="15"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="38"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="33"/>
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="15"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="38"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="33"/>
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="38"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="33"/>
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="15"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="37"/>
-      <c r="R26" s="37"/>
-      <c r="S26" s="38"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="33"/>
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="15"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="38"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="33"/>
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="27"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="38"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="33"/>
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="28"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="40"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="35"/>
     </row>
     <row r="30" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
@@ -2162,6 +2186,27 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="B9:S9"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="S12:S14"/>
@@ -2176,28 +2221,7 @@
     <mergeCell ref="D10:J11"/>
     <mergeCell ref="K10:N11"/>
     <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="O11:O14"/>
     <mergeCell ref="P11:P14"/>
-    <mergeCell ref="Q12:Q14"/>
-    <mergeCell ref="R12:R14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>